<commit_message>
cours de queli dev
</commit_message>
<xml_diff>
--- a/proba/tp2/Classeur1.xlsx
+++ b/proba/tp2/Classeur1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\cours2\proba\tp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514D495E-65EA-4C02-8B09-F4CE5C30960C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB1B62F-B5B0-4E14-A065-4101E3CE1EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{FC34F5CD-025D-49D6-A3DD-F83FE0D579AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC34F5CD-025D-49D6-A3DD-F83FE0D579AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>xi</t>
   </si>
@@ -125,13 +125,28 @@
   <si>
     <t>p(Y=xi)</t>
   </si>
+  <si>
+    <t>EXO 12</t>
+  </si>
+  <si>
+    <t>simulation d'une loi uniforme discrete sur {1,2,3,4,5,6)</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>somme :</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -149,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +174,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,8 +212,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3817,15 +3826,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905122DF-A6F6-4AF9-AC44-2D8DC116BA9B}">
-  <dimension ref="A2:BA94"/>
+  <dimension ref="A2:BA105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="53" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4873,8 +4884,118 @@
         <v>1.9676730382787648E-32</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97">
+        <f ca="1">RAND()</f>
+        <v>0.72715865376314559</v>
+      </c>
+      <c r="D97" s="6">
+        <f ca="1">IF(B97&lt;1/6,1,IF(B97&lt;2/6,2,IF(B97&lt;3/6,3,IF(B97&lt;4/6,4,IF(B97&lt;5/6,5,6)))))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2</v>
+      </c>
+      <c r="F101" s="1">
+        <v>3</v>
+      </c>
+      <c r="G101" s="1">
+        <v>4</v>
+      </c>
+      <c r="H101" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1">
+        <f>BINOMDIST(C101,5,0.2,0)</f>
+        <v>0.32768000000000003</v>
+      </c>
+      <c r="D102" s="1">
+        <f t="shared" ref="D102:H102" si="8">BINOMDIST(D101,5,0.2,0)</f>
+        <v>0.40959999999999996</v>
+      </c>
+      <c r="E102" s="1">
+        <f t="shared" si="8"/>
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="F102" s="1">
+        <f t="shared" si="8"/>
+        <v>5.1199999999999996E-2</v>
+      </c>
+      <c r="G102" s="1">
+        <f t="shared" si="8"/>
+        <v>6.4000000000000029E-3</v>
+      </c>
+      <c r="H102" s="1">
+        <f t="shared" si="8"/>
+        <v>3.2000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <f ca="1">IF(RAND()&lt;0.2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <f t="shared" ref="D105:H105" ca="1" si="9">IF(RAND()&lt;0.2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J105" t="s">
+        <v>34</v>
+      </c>
+      <c r="K105">
+        <f ca="1">C105+D105+E105+F105+G105+H105</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>